<commit_message>
RPA-93:Lage intitieringsfil og rutine
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v1.0.xlsx
+++ b/Vasklister/Excel/vaskeliste_v1.0.xlsx
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>_1_inntekt</t>
   </si>
   <si>
     <t>_1_isProcentTrekk</t>
@@ -81,10 +78,13 @@
     <t>_4_barnetrygd</t>
   </si>
   <si>
-    <t>13088334935</t>
+    <t>Kommune_Nr</t>
   </si>
   <si>
-    <t>267794</t>
+    <t>13098245418</t>
+  </si>
+  <si>
+    <t>313054</t>
   </si>
 </sst>
 </file>
@@ -453,58 +453,58 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ainntekt tar nå høyde for de med pensjon fra kun ett sted.
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v1.0.xlsx
+++ b/Vasklister/Excel/vaskeliste_v1.0.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="22">
   <si>
     <t>debitor_ident</t>
   </si>
@@ -81,10 +81,7 @@
     <t>Kommune_Nr</t>
   </si>
   <si>
-    <t>13098245418</t>
-  </si>
-  <si>
-    <t>313054</t>
+    <t>_1_inntekt</t>
   </si>
 </sst>
 </file>
@@ -120,12 +117,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T300"/>
+  <dimension ref="A1:U300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,14 +437,15 @@
     <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,345 +455,433 @@
       <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>13088334935</v>
+      </c>
+      <c r="B2" s="3">
+        <v>267794</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3">
+        <v>13088334935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>13098245418</v>
+      </c>
+      <c r="B3" s="3">
+        <v>313054</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
+        <v>13098245418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>13098946823</v>
+      </c>
+      <c r="B4" s="3">
+        <v>239603</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3">
+        <v>13098946823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>13099148734</v>
+      </c>
+      <c r="B5" s="3">
+        <v>315219</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3">
+        <v>13099148734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>13128239213</v>
+      </c>
+      <c r="B6" s="3">
+        <v>302246</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3">
+        <v>13128239213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>13128848074</v>
+      </c>
+      <c r="B7" s="3">
+        <v>253876</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3">
+        <v>13128848074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>14018247195</v>
+      </c>
+      <c r="B8" s="3">
+        <v>225869</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3">
+        <v>14018247195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>14018247195</v>
+      </c>
+      <c r="B9" s="3">
+        <v>225870</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3">
+        <v>14018247195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>14018247195</v>
+      </c>
+      <c r="B10" s="3">
+        <v>260250</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3">
+        <v>14018247195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>14026844259</v>
+      </c>
+      <c r="B11" s="3">
+        <v>291551</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3">
+        <v>14026844259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>14026844259</v>
+      </c>
+      <c r="B12" s="3">
+        <v>292217</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3">
+        <v>14026844259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>14028147164</v>
+      </c>
+      <c r="B13" s="3">
+        <v>207756</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3">
+        <v>14028147164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>14028739460</v>
+      </c>
+      <c r="B14" s="3">
+        <v>307204</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3">
+        <v>14028739460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14028739460</v>
+      </c>
+      <c r="B15" s="3">
+        <v>307205</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3">
+        <v>14028739460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14035931717</v>
+      </c>
+      <c r="B16" s="3">
+        <v>260129</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3">
+        <v>14035931717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>14036749548</v>
+      </c>
+      <c r="B17" s="3">
+        <v>159700</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3">
+        <v>14036749548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>14056445049</v>
+      </c>
+      <c r="B18" s="3">
+        <v>211756</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3">
+        <v>14056445049</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>14078833085</v>
+      </c>
+      <c r="B19" s="3">
+        <v>313856</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3">
+        <v>14078833085</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>14087022758</v>
+      </c>
+      <c r="B20" s="3">
+        <v>256613</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3">
+        <v>14087022758</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>14087128378</v>
+      </c>
+      <c r="B21" s="3">
+        <v>302060</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3">
+        <v>14087128378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>14118829396</v>
+      </c>
+      <c r="B22" s="3">
+        <v>203314</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3">
+        <v>14118829396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>15015026399</v>
+      </c>
+      <c r="B23" s="3">
+        <v>52338</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3">
+        <v>15015026399</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>15018334116</v>
+      </c>
+      <c r="B24" s="3">
+        <v>131251</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3">
+        <v>15018334116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>15027529981</v>
+      </c>
+      <c r="B25" s="3">
+        <v>245984</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3">
+        <v>15027529981</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
@@ -804,7 +892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -815,7 +903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -826,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -837,7 +925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Fjernet ubrukt kode i aInntekt samt ubrukte kommentarer.
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v1.0.xlsx
+++ b/Vasklister/Excel/vaskeliste_v1.0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="22">
   <si>
     <t>debitor_ident</t>
   </si>
@@ -429,7 +429,7 @@
   <dimension ref="A1:U300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,319 +554,151 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>13099148734</v>
-      </c>
-      <c r="B5" s="3">
-        <v>315219</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="3">
-        <v>13099148734</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>13128239213</v>
-      </c>
-      <c r="B6" s="3">
-        <v>302246</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="3">
-        <v>13128239213</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>13128848074</v>
-      </c>
-      <c r="B7" s="3">
-        <v>253876</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="3">
-        <v>13128848074</v>
-      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>14018247195</v>
-      </c>
-      <c r="B8" s="3">
-        <v>225869</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="3">
-        <v>14018247195</v>
-      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>14018247195</v>
-      </c>
-      <c r="B9" s="3">
-        <v>225870</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="3">
-        <v>14018247195</v>
-      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>14018247195</v>
-      </c>
-      <c r="B10" s="3">
-        <v>260250</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="3">
-        <v>14018247195</v>
-      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>14026844259</v>
-      </c>
-      <c r="B11" s="3">
-        <v>291551</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="3">
-        <v>14026844259</v>
-      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>14026844259</v>
-      </c>
-      <c r="B12" s="3">
-        <v>292217</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="3">
-        <v>14026844259</v>
-      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>14028147164</v>
-      </c>
-      <c r="B13" s="3">
-        <v>207756</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="3">
-        <v>14028147164</v>
-      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>14028739460</v>
-      </c>
-      <c r="B14" s="3">
-        <v>307204</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="3">
-        <v>14028739460</v>
-      </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14028739460</v>
-      </c>
-      <c r="B15" s="3">
-        <v>307205</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="3">
-        <v>14028739460</v>
-      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>14035931717</v>
-      </c>
-      <c r="B16" s="3">
-        <v>260129</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="3">
-        <v>14035931717</v>
-      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>14036749548</v>
-      </c>
-      <c r="B17" s="3">
-        <v>159700</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="3">
-        <v>14036749548</v>
-      </c>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>14056445049</v>
-      </c>
-      <c r="B18" s="3">
-        <v>211756</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="3">
-        <v>14056445049</v>
-      </c>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>14078833085</v>
-      </c>
-      <c r="B19" s="3">
-        <v>313856</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="3">
-        <v>14078833085</v>
-      </c>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>14087022758</v>
-      </c>
-      <c r="B20" s="3">
-        <v>256613</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="3">
-        <v>14087022758</v>
-      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>14087128378</v>
-      </c>
-      <c r="B21" s="3">
-        <v>302060</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="3">
-        <v>14087128378</v>
-      </c>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>14118829396</v>
-      </c>
-      <c r="B22" s="3">
-        <v>203314</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="3">
-        <v>14118829396</v>
-      </c>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>15015026399</v>
-      </c>
-      <c r="B23" s="3">
-        <v>52338</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="3">
-        <v>15015026399</v>
-      </c>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>15018334116</v>
-      </c>
-      <c r="B24" s="3">
-        <v>131251</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="3">
-        <v>15018334116</v>
-      </c>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>15027529981</v>
-      </c>
-      <c r="B25" s="3">
-        <v>245984</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="3">
-        <v>15027529981</v>
-      </c>
+      <c r="E25" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">

</xml_diff>

<commit_message>
Navn endring på Main i del2 til del2Main for å slippe fremtidig forvirring.
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v1.0.xlsx
+++ b/Vasklister/Excel/vaskeliste_v1.0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="41">
   <si>
     <t>debitor_ident</t>
   </si>
@@ -487,7 +487,7 @@
   <dimension ref="A1:U300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,17 +570,377 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>14048929681</v>
+        <v>13088334935</v>
       </c>
       <c r="B2" s="3">
-        <v>309647</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>267794</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3">
+        <v>13088334935</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>13098245418</v>
+      </c>
+      <c r="B3" s="3">
+        <v>313054</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
+        <v>13098245418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>13098946823</v>
+      </c>
+      <c r="B4" s="3">
+        <v>239603</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3">
+        <v>13098946823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>13099148734</v>
+      </c>
+      <c r="B5" s="3">
+        <v>315219</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3">
+        <v>13099148734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>13128239213</v>
+      </c>
+      <c r="B6" s="3">
+        <v>302246</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3">
+        <v>13128239213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>13128848074</v>
+      </c>
+      <c r="B7" s="3">
+        <v>253876</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3">
+        <v>13128848074</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>14018247195</v>
+      </c>
+      <c r="B8" s="3">
+        <v>225869</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3">
+        <v>14018247195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>14018247195</v>
+      </c>
+      <c r="B9" s="3">
+        <v>225870</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3">
+        <v>14018247195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>14018247195</v>
+      </c>
+      <c r="B10" s="3">
+        <v>260250</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3">
+        <v>14018247195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>14026844259</v>
+      </c>
+      <c r="B11" s="3">
+        <v>291551</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3">
+        <v>14026844259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>14026844259</v>
+      </c>
+      <c r="B12" s="3">
+        <v>292217</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3">
+        <v>14026844259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>14028147164</v>
+      </c>
+      <c r="B13" s="3">
+        <v>207756</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3">
+        <v>14028147164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>14028739460</v>
+      </c>
+      <c r="B14" s="3">
+        <v>307204</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3">
+        <v>14028739460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14028739460</v>
+      </c>
+      <c r="B15" s="3">
+        <v>307205</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3">
+        <v>14028739460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14035931717</v>
+      </c>
+      <c r="B16" s="3">
+        <v>260129</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3">
+        <v>14035931717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>14036749548</v>
+      </c>
+      <c r="B17" s="3">
+        <v>159700</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3">
+        <v>14036749548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>14048929681</v>
+      </c>
+      <c r="B18" s="3">
+        <v>309647</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3">
+        <v>14048929681</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>14056445049</v>
+      </c>
+      <c r="B19" s="3">
+        <v>211756</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3">
+        <v>14056445049</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>14078833085</v>
+      </c>
+      <c r="B20" s="3">
+        <v>313856</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3">
+        <v>14078833085</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>14087022758</v>
+      </c>
+      <c r="B21" s="3">
+        <v>256613</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3">
+        <v>14087022758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>14087128378</v>
+      </c>
+      <c r="B22" s="3">
+        <v>302060</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3">
+        <v>14087128378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>14118829396</v>
+      </c>
+      <c r="B23" s="3">
+        <v>203314</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3">
+        <v>14118829396</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>15015026399</v>
+      </c>
+      <c r="B24" s="3">
+        <v>52338</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3">
+        <v>15015026399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>15018334116</v>
+      </c>
+      <c r="B25" s="3">
+        <v>131251</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3">
+        <v>15018334116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>15027529981</v>
+      </c>
+      <c r="B26" s="3">
+        <v>245984</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3">
+        <v>15027529981</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3591,7 +3951,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+      <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>